<commit_message>
fixed clearing values for kard
</commit_message>
<xml_diff>
--- a/UnitTests/Excel/Testfiles/unnested_attributes_clear_values.xlsx
+++ b/UnitTests/Excel/Testfiles/unnested_attributes_clear_values.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t xml:space="preserve">typeURI</t>
   </si>
@@ -80,12 +80,6 @@
   </si>
   <si>
     <t xml:space="preserve">0000-0000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">88888888.0|88888888.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">88888888|88888888 </t>
   </si>
 </sst>
 </file>
@@ -95,7 +89,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -117,12 +111,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -172,7 +160,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -196,10 +184,10 @@
   <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F:F"/>
+      <selection pane="topLeft" activeCell="R2" activeCellId="0" sqref="R2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.17"/>
@@ -287,8 +275,8 @@
       <c r="H2" s="1" t="n">
         <v>88888888</v>
       </c>
-      <c r="I2" s="0" t="s">
-        <v>20</v>
+      <c r="I2" s="0" t="n">
+        <v>88888888</v>
       </c>
       <c r="J2" s="1" t="n">
         <v>88888888</v>
@@ -296,8 +284,8 @@
       <c r="K2" s="1" t="n">
         <v>88888888</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>21</v>
+      <c r="L2" s="1" t="n">
+        <v>88888888</v>
       </c>
       <c r="M2" s="1" t="n">
         <v>88888888</v>
@@ -311,8 +299,8 @@
       <c r="P2" s="1" t="n">
         <v>88888888</v>
       </c>
-      <c r="Q2" s="1" t="s">
-        <v>21</v>
+      <c r="Q2" s="1" t="n">
+        <v>88888888</v>
       </c>
       <c r="R2" s="1" t="n">
         <v>88888888</v>

</xml_diff>